<commit_message>
Update to include example Dataset.jsonld and mapping table from DMAS Solr Response to JSON-LD Dataset.json object
</commit_message>
<xml_diff>
--- a/dmas_solr_to_schema_dot_org_mapping.xlsx
+++ b/dmas_solr_to_schema_dot_org_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmcgibbn/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmcgibbn/Downloads/podaac.geosci.schema.org/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5FDA549-4F10-A941-B859-7F5E7F82BA74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF834C6-E170-9042-93E3-C5E4185ADA3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{254D5264-42DF-3140-A100-587E8225166B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>DMAS Solr Key</t>
   </si>
@@ -178,13 +178,91 @@
   </si>
   <si>
     <t>We need to set up a small map here to read the Solr DMAS value and map it to the formal IANA Mime Type.</t>
+  </si>
+  <si>
+    <t>temporalCoverage</t>
+  </si>
+  <si>
+    <t>spatialCoverage</t>
+  </si>
+  <si>
+    <t>Dataset-DatasetCoverage-StartTimeLong + "/" + Dataset-DatasetCoverage-StopTimeLong</t>
+  </si>
+  <si>
+    <t>Temporal coverage at PO.DAAC is always defined using a date range e.g. 2012-09-20 - 2016-01-22 for example. The datetime needs to be mapped from the Long datetime included within the DMAS Solr response to the ISO 8601 equivalent. Additionally, if the end time is present or ongoing, then the datetime range can be expressed as follows "2012-09-20/.." note the two dots in the end date entry. This is documented further at https://github.com/schemaorg/schemaorg/issues/242. Also note, that the DMAS Solr response includes three varieties of start time e.g. DatasetCoverage-StartTimeLong-Long and DatasetCoverage-StartTimeLong in addition to Dataset-DatasetCoverage-StartTimeLong. The same is true for end times.</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-dataset</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-dataset-identifier</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-variables</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-distributions</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-temporal-coverage</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-spatial-coverage</t>
+  </si>
+  <si>
+    <t>This is always represented as a schema.org/Place of type GeoShape of type 'box'. See the accompanying Dataset.jsonld document for an example. In the example provided the 'lower-left' corner is 39.3280/120.1633 and 'upper-right' corner is 40.445/123.7878</t>
+  </si>
+  <si>
+    <t>DatasetCoverage-NorthLat, DatasetCoverage-SouthLat, DatasetCoverage-WestLon, DatasetCoverage-EastLon</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Descrbing a datasets people is not particularly of interest to PO.DAAC. The reason here is that we do not necessarily wish for people included in the DMAS Solr response to be stated as points of contact for the PO.DAAC dataset.</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-people</t>
+  </si>
+  <si>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#describing-a-datasets-publisherprovider</t>
+  </si>
+  <si>
+    <t>Same as for DataRepository, this value is is simply 'https://podaac.jpl.nasa.gov'</t>
+  </si>
+  <si>
+    <t>additionalProperty</t>
+  </si>
+  <si>
+    <t>Dataset-EllipsoidType</t>
+  </si>
+  <si>
+    <t>See the example for how one would map a value to CRS84. Lot's of the PO.DAAC Datasets have WGS84 ellipsoid representations however, so we need to map those differently. See both the science-on-schema.org link and the Dataset.json example.</t>
+  </si>
+  <si>
+    <t>https://github.com/ESIPFed/science-on-schema.org/blob/master/guides/Dataset.md#spatial_multiple-geometries</t>
+  </si>
+  <si>
+    <t>DatasetFunding</t>
+  </si>
+  <si>
+    <t>Same as with 'creator' we most likely do NOT wish to go into details of who funded the dataset. Right now, I don't think we host that kind of information at PO.DAAC right now anyway. This is another open question however.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +274,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,10 +304,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -230,8 +317,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C944F2-950C-5246-AB33-10417DA7D58B}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,7 +646,7 @@
     <col min="3" max="3" width="94" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,8 +656,11 @@
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -578,16 +670,22 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -597,8 +695,11 @@
       <c r="C4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -608,16 +709,22 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -627,16 +734,22 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -646,64 +759,88 @@
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -713,24 +850,33 @@
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -740,8 +886,11 @@
       <c r="C20" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -752,12 +901,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>46</v>
       </c>
@@ -767,8 +919,11 @@
       <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -778,8 +933,103 @@
       <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" location="describing-a-datasets-variables" xr:uid="{9ADAA019-BA31-6341-8C6F-AA092F1711AA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mapping based on feedback from 2nd schema.org workshop
</commit_message>
<xml_diff>
--- a/dmas_solr_to_schema_dot_org_mapping.xlsx
+++ b/dmas_solr_to_schema_dot_org_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmcgibbn/Downloads/podaac.geosci.schema.org/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF834C6-E170-9042-93E3-C5E4185ADA3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0BC959-5428-6142-AA28-97F4C464A686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{254D5264-42DF-3140-A100-587E8225166B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>DMAS Solr Key</t>
   </si>
@@ -75,9 +75,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Theres a possibility we could construct the dataset landing page URL here</t>
-  </si>
-  <si>
     <t>DatasetCitation-Version</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Same as schema.org 'url' mapping</t>
   </si>
   <si>
-    <t>If Dataset-Doi is not available try Dataset-SecondaryDoi. Any value need to be prepended with 'https://doi.org/'</t>
-  </si>
-  <si>
     <t>Although the values for the nested object are the same as schema.org 'url' mapping there are some notable intricacies.</t>
   </si>
   <si>
@@ -256,6 +250,15 @@
   </si>
   <si>
     <t>Same as with 'creator' we most likely do NOT wish to go into details of who funded the dataset. Right now, I don't think we host that kind of information at PO.DAAC right now anyway. This is another open question however.</t>
+  </si>
+  <si>
+    <t>If Dataset-Doi is not available try Dataset-SecondaryDoi. Any value needs to be prepended with 'https://dx.doi.org/'</t>
+  </si>
+  <si>
+    <t>Theres a possibility we could construct the dataset landing page URL here. The logic would therefore be 'https://podaac.jpl.nasa.gov/dataset/' + Dataset Shortname e.g. 'UPA-L2P-ATS_NR_2P'</t>
+  </si>
+  <si>
+    <t>Do we want to flag to PO.DAAC Data Engineering that Variable descriptors are lacking???</t>
   </si>
 </sst>
 </file>
@@ -635,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C944F2-950C-5246-AB33-10417DA7D58B}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -671,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -682,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -693,13 +696,13 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -707,21 +710,21 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -732,21 +735,21 @@
         <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -757,87 +760,90 @@
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -845,24 +851,24 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -870,24 +876,24 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -895,99 +901,99 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" t="s">
         <v>64</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -995,13 +1001,13 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1009,21 +1015,21 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>